<commit_message>
added more expenses to the excel file
</commit_message>
<xml_diff>
--- a/ExpenseTrackingApp/ExcelFiles/MyExpenses.xlsx
+++ b/ExpenseTrackingApp/ExcelFiles/MyExpenses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruslan\Desktop\Git_test\CustomProjects\ExpenseTrackingApp\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875880FD-3150-47B3-A6AA-968CD4BE0AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93702BC0-08C3-47C1-8EE5-A70A3674BF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -118,20 +118,98 @@
     <t>Ruslan</t>
   </si>
   <si>
-    <t>Credit Card BofA</t>
+    <t>Credit Card BofA 8484</t>
+  </si>
+  <si>
+    <t>Kids</t>
+  </si>
+  <si>
+    <t>Lego Oak Park Mall</t>
+  </si>
+  <si>
+    <t>Buldozer</t>
+  </si>
+  <si>
+    <t>Carter's Shawnee Mission Pkway</t>
+  </si>
+  <si>
+    <t>Boys Knit Top</t>
+  </si>
+  <si>
+    <t>Farida</t>
+  </si>
+  <si>
+    <t>Credit Card BofA 2694</t>
+  </si>
+  <si>
+    <t>Walmart Frontage Road Overland Park</t>
+  </si>
+  <si>
+    <t>Glue All Purpose</t>
+  </si>
+  <si>
+    <t>Scissor</t>
+  </si>
+  <si>
+    <t>PC Mouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bar Soap </t>
+  </si>
+  <si>
+    <t>Play snake</t>
+  </si>
+  <si>
+    <t>Bush</t>
+  </si>
+  <si>
+    <t>Walmart 74th Terrace Shawnee</t>
+  </si>
+  <si>
+    <t>JJ Aples bag</t>
+  </si>
+  <si>
+    <t>Potatoes</t>
+  </si>
+  <si>
+    <t>Tomato Roma</t>
+  </si>
+  <si>
+    <t>Tomato Souce</t>
+  </si>
+  <si>
+    <t>Tomato Juice</t>
+  </si>
+  <si>
+    <t>Avocado</t>
+  </si>
+  <si>
+    <t>Garlic</t>
+  </si>
+  <si>
+    <t>Peper Anaheim</t>
+  </si>
+  <si>
+    <t>Pepper Bell</t>
+  </si>
+  <si>
+    <t>White Kidney Beans</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,9 +235,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -442,17 +519,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
     <col min="4" max="4" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -480,7 +557,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>44406</v>
       </c>
       <c r="B2">
@@ -498,13 +575,13 @@
       <c r="F2">
         <v>2.89</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <f>E2*F2</f>
         <v>2.89</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>44406</v>
       </c>
       <c r="B3">
@@ -522,13 +599,13 @@
       <c r="F3">
         <v>1.99</v>
       </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G14" si="0">E3*F3</f>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G12" si="0">E3*F3</f>
         <v>1.99</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>44406</v>
       </c>
       <c r="B4">
@@ -546,13 +623,13 @@
       <c r="F4">
         <v>2.25</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>44406</v>
       </c>
       <c r="B5">
@@ -570,13 +647,13 @@
       <c r="F5">
         <v>1.49</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <f t="shared" si="0"/>
         <v>2.9203999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>44406</v>
       </c>
       <c r="B6">
@@ -594,13 +671,13 @@
       <c r="F6">
         <v>0.36</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <f t="shared" si="0"/>
         <v>0.50039999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>44406</v>
       </c>
       <c r="B7">
@@ -618,13 +695,13 @@
       <c r="F7">
         <v>1.29</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>1.29</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>44406</v>
       </c>
       <c r="B8">
@@ -642,13 +719,13 @@
       <c r="F8">
         <v>1.49</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <f t="shared" si="0"/>
         <v>1.49</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>44406</v>
       </c>
       <c r="B9">
@@ -666,13 +743,13 @@
       <c r="F9">
         <v>0.95</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <f t="shared" si="0"/>
         <v>2.7645</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>44406</v>
       </c>
       <c r="B10">
@@ -690,13 +767,13 @@
       <c r="F10">
         <v>0.75</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>44406</v>
       </c>
       <c r="B11">
@@ -714,13 +791,13 @@
       <c r="F11">
         <v>4.79</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <f t="shared" si="0"/>
         <v>4.79</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>44406</v>
       </c>
       <c r="B12">
@@ -738,13 +815,13 @@
       <c r="F12">
         <v>1.25</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>44406</v>
       </c>
       <c r="B13">
@@ -756,35 +833,622 @@
       <c r="D13" t="s">
         <v>19</v>
       </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
       <c r="F13">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <f>SUM(G2:G12)*F13</f>
         <v>2.1963122999999998</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="G14" s="3"/>
+      <c r="A14" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B14">
+        <v>46277</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>9.99</v>
+      </c>
+      <c r="G14" s="2">
+        <f>E14*F14</f>
+        <v>9.99</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1">
+        <v>44354</v>
+      </c>
+      <c r="B15">
+        <v>46277</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="G15" s="2">
+        <f>F15*F14</f>
+        <v>0.95904</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
+      <c r="A16" s="1">
+        <v>44079</v>
+      </c>
+      <c r="B16">
+        <v>31568</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <f>E16*F16</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44079</v>
+      </c>
+      <c r="B17">
+        <v>31568</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="G17" s="2">
+        <f>F17*G16</f>
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B18">
+        <v>1299</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1.26</v>
+      </c>
+      <c r="G18">
+        <f>E18*F18</f>
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B19">
+        <v>1299</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1.88</v>
+      </c>
+      <c r="G19">
+        <f>E19*F19</f>
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B20">
+        <v>1299</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="G20" s="2">
+        <f>(G18+G19)*F20</f>
+        <v>0.28573999999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44346</v>
+      </c>
+      <c r="B21">
+        <v>992</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>12.88</v>
+      </c>
+      <c r="G21">
+        <f>E21*F21</f>
+        <v>12.88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>44346</v>
+      </c>
+      <c r="B22">
+        <v>992</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>3.97</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ref="G22:G24" si="1">E22*F22</f>
+        <v>3.97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>44346</v>
+      </c>
+      <c r="B23">
+        <v>992</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>44346</v>
+      </c>
+      <c r="B24">
+        <v>992</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0.97</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>44346</v>
+      </c>
+      <c r="B25">
+        <v>992</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="G25" s="2">
+        <f>(G21+G22+G23+G24)*F25</f>
+        <v>1.71262</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B26">
+        <v>4052</v>
+      </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>2.46</v>
+      </c>
+      <c r="G26" s="2">
+        <f>E26*F26</f>
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B27">
+        <v>4052</v>
+      </c>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27">
+        <v>3.37</v>
+      </c>
+      <c r="F27">
+        <v>0.68</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" ref="G27:G37" si="2">E27*F27</f>
+        <v>2.2916000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B28">
+        <v>4052</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28">
+        <v>1.03</v>
+      </c>
+      <c r="F28">
+        <v>1.92</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="2"/>
+        <v>1.9776</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B29">
+        <v>4052</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="F29">
+        <v>0.98</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0682</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>44535</v>
+      </c>
+      <c r="B30">
+        <v>4053</v>
+      </c>
+      <c r="C30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B31">
+        <v>4052</v>
+      </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0.98</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="2"/>
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B32">
+        <v>4052</v>
+      </c>
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="2"/>
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B33">
+        <v>4052</v>
+      </c>
+      <c r="C33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>0.78</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="2"/>
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B34">
+        <v>4052</v>
+      </c>
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34">
+        <v>0.24</v>
+      </c>
+      <c r="F34">
+        <v>3.81</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="2"/>
+        <v>0.91439999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B35">
+        <v>4052</v>
+      </c>
+      <c r="C35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35">
+        <v>0.15</v>
+      </c>
+      <c r="F35">
+        <v>2.58</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="2"/>
+        <v>0.38700000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B36">
+        <v>4052</v>
+      </c>
+      <c r="C36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0.78</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="2"/>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B37">
+        <v>4052</v>
+      </c>
+      <c r="C37" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37">
+        <v>1.68</v>
+      </c>
+      <c r="F37">
+        <v>0.59</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="2"/>
+        <v>0.99119999999999986</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B38">
+        <v>4052</v>
+      </c>
+      <c r="C38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="G38" s="2">
+        <f>SUM(G26:G37)*F38</f>
+        <v>1.5542400000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -793,17 +1457,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2772B062-4FC8-46CB-BC02-99E8E766A8D0}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G20:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.77734375" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -841,7 +1505,93 @@
         <v>26.33</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>46277</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3">
+        <v>10.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>31568</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1299</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5">
+        <v>3.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>992</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6">
+        <v>20.53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4052</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7">
+        <v>17.739999999999998</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added some new expenses
</commit_message>
<xml_diff>
--- a/ExpenseTrackingApp/ExcelFiles/MyExpenses.xlsx
+++ b/ExpenseTrackingApp/ExcelFiles/MyExpenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruslan\Desktop\Git_test\CustomProjects\ExpenseTrackingApp\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93702BC0-08C3-47C1-8EE5-A70A3674BF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9642BE7-113D-4EF1-9872-179FC59BE33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1460,7 +1460,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G20:G21"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>